<commit_message>
Results with also Kappa metric
</commit_message>
<xml_diff>
--- a/Results_2A/Results_Z_Score_unique/Results_SegRec/Results_Cross/Results_MSVT_SE_SE_Net/seed_results_MSVT_SE_SE_Net.xlsx
+++ b/Results_2A/Results_Z_Score_unique/Results_SegRec/Results_Cross/Results_MSVT_SE_SE_Net/seed_results_MSVT_SE_SE_Net.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -533,7 +533,7 @@
         <v>0.83</v>
       </c>
       <c r="C3" t="n">
-        <v>0.604</v>
+        <v>0.601</v>
       </c>
       <c r="D3" t="n">
         <v>0.9379999999999999</v>
@@ -557,7 +557,7 @@
         <v>0.76</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7752222222222221</v>
+        <v>0.774888888888889</v>
       </c>
     </row>
     <row r="4">
@@ -743,7 +743,7 @@
         <v>0.837</v>
       </c>
       <c r="C9" t="n">
-        <v>0.58</v>
+        <v>0.583</v>
       </c>
       <c r="D9" t="n">
         <v>0.955</v>
@@ -767,7 +767,7 @@
         <v>0.774</v>
       </c>
       <c r="K9" t="n">
-        <v>0.7527777777777778</v>
+        <v>0.7531111111111111</v>
       </c>
     </row>
     <row r="10">

</xml_diff>